<commit_message>
first successful sample excel parse and insert to db.
</commit_message>
<xml_diff>
--- a/uploaded/MOCK_DATA_short.xlsx
+++ b/uploaded/MOCK_DATA_short.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15615" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>sampleId</t>
   </si>
@@ -87,21 +87,6 @@
     <t>diseaseFreeText</t>
   </si>
   <si>
-    <t>187912434-3</t>
-  </si>
-  <si>
-    <t>faucibus orci luctus et ultrices posuere cubilia curae duis faucibus accumsan odio curabitur convallis duis</t>
-  </si>
-  <si>
-    <t>fusce congue diam id ornare imperdiet sapien urna pretium nisl ut volutpat sapien arcu</t>
-  </si>
-  <si>
-    <t>nam congue risus semper porta volutpat quam pede lobortis ligula sit amet</t>
-  </si>
-  <si>
-    <t>6/28/2014</t>
-  </si>
-  <si>
     <t>Aenean lectus. Pellentesque eget nunc. Donec quis orci eget orci vehicula condimentum.</t>
   </si>
   <si>
@@ -109,21 +94,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>301778537-8</t>
-  </si>
-  <si>
-    <t>nulla suspendisse potenti cras in purus eu magna vulputate luctus cum</t>
-  </si>
-  <si>
-    <t>justo etiam pretium iaculis justo in hac habitasse platea dictumst etiam faucibus</t>
-  </si>
-  <si>
-    <t>quisque porta volutpat erat quisque erat eros viverra eget congue eget semper rutrum nulla nunc purus phasellus in</t>
-  </si>
-  <si>
-    <t>12/4/2014</t>
   </si>
   <si>
     <t>Quisque id justo sit amet sapien dignissim vestibulum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Nulla dapibus dolor vel est. Donec odio justo, sollicitudin ut, suscipit a, feugiat et, eros.
@@ -134,21 +104,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>073010831-7</t>
-  </si>
-  <si>
-    <t>phasellus in felis donec semper sapien a libero nam dui proin leo odio porttitor id consequat in consequat ut nulla</t>
-  </si>
-  <si>
-    <t>ut mauris eget massa tempor convallis nulla neque libero convallis eget eleifend luctus ultricies eu nibh quisque</t>
-  </si>
-  <si>
-    <t>magna bibendum imperdiet nullam orci pede venenatis non sodales sed tincidunt</t>
-  </si>
-  <si>
-    <t>6/29/2014</t>
-  </si>
-  <si>
     <t>Integer tincidunt ante vel ipsum. Praesent blandit lacinia erat. Vestibulum sed magna at nunc commodo placerat.
 Praesent blandit. Nam nulla. Integer pede justo, lacinia eget, tincidunt eget, tempus vel, pede.
 Morbi porttitor lorem id ligula. Suspendisse ornare consequat lectus. In est risus, auctor sed, tristique in, tempus sit amet, sem.</t>
@@ -158,60 +113,15 @@
 Cras non velit nec nisi vulputate nonummy. Maecenas tincidunt lacus at velit. Vivamus vel nulla eget eros elementum pellentesque.</t>
   </si>
   <si>
-    <t>843173078-1</t>
-  </si>
-  <si>
-    <t>accumsan tellus nisi eu orci mauris lacinia sapien quis libero nullam sit amet turpis elementum ligula</t>
-  </si>
-  <si>
-    <t>id nisl venenatis lacinia aenean sit amet justo morbi ut odio cras mi pede malesuada in imperdiet et</t>
-  </si>
-  <si>
-    <t>proin risus praesent lectus vestibulum quam sapien varius ut blandit non interdum in ante vestibulum ante ipsum primis</t>
-  </si>
-  <si>
-    <t>10/11/2014</t>
-  </si>
-  <si>
     <t>Etiam vel augue. Vestibulum rutrum rutrum neque. Aenean auctor gravida sem.
 Praesent id massa id nisl venenatis lacinia. Aenean sit amet justo. Morbi ut odio.
 Cras mi pede, malesuada in, imperdiet et, commodo vulputate, justo. In blandit ultrices enim. Lorem ipsum dolor sit amet, consectetuer adipiscing elit.</t>
   </si>
   <si>
-    <t>973721305-X</t>
-  </si>
-  <si>
-    <t>in imperdiet et commodo vulputate justo in blandit ultrices enim lorem</t>
-  </si>
-  <si>
-    <t>dolor vel est donec odio justo sollicitudin ut suscipit a feugiat et eros</t>
-  </si>
-  <si>
-    <t>sagittis dui vel nisl duis ac nibh fusce lacus purus aliquet at feugiat non pretium</t>
-  </si>
-  <si>
-    <t>11/6/2014</t>
-  </si>
-  <si>
     <t>Curabitur in libero ut massa volutpat convallis. Morbi odio odio, elementum eu, interdum eu, tincidunt in, leo. Maecenas pulvinar lobortis est.</t>
   </si>
   <si>
     <t>Nullam porttitor lacus at turpis. Donec posuere metus vitae ipsum. Aliquam non mauris.</t>
-  </si>
-  <si>
-    <t>696556734-1</t>
-  </si>
-  <si>
-    <t>luctus tincidunt nulla mollis molestie lorem quisque ut erat curabitur gravida nisi at nibh in</t>
-  </si>
-  <si>
-    <t>massa donec dapibus duis at velit eu est congue elementum in hac</t>
-  </si>
-  <si>
-    <t>dictumst morbi vestibulum velit id pretium iaculis diam erat fermentum justo nec condimentum neque sapien placerat ante nulla justo aliquam</t>
-  </si>
-  <si>
-    <t>6/9/2014</t>
   </si>
   <si>
     <t>Maecenas tristique, est et tempus semper, est quam pharetra magna, ac consequat metus sapien ut nunc. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Mauris viverra diam vitae quam. Suspendisse potenti.
@@ -223,40 +133,10 @@
 Fusce consequat. Nulla nisl. Nunc nisl.</t>
   </si>
   <si>
-    <t>983007598-2</t>
-  </si>
-  <si>
-    <t>platea dictumst morbi vestibulum velit id pretium iaculis diam erat fermentum justo nec</t>
-  </si>
-  <si>
-    <t>amet eros suspendisse accumsan tortor quis turpis sed ante vivamus tortor duis mattis egestas metus aenean fermentum donec ut</t>
-  </si>
-  <si>
-    <t>morbi a ipsum integer a nibh in quis justo maecenas rhoncus aliquam lacus morbi quis tortor id nulla ultrices</t>
-  </si>
-  <si>
-    <t>11/1/2014</t>
-  </si>
-  <si>
     <t>In quis justo. Maecenas rhoncus aliquam lacus. Morbi quis tortor id nulla ultrices aliquet.</t>
   </si>
   <si>
     <t>In hac habitasse platea dictumst. Morbi vestibulum, velit id pretium iaculis, diam erat fermentum justo, nec condimentum neque sapien placerat ante. Nulla justo.</t>
-  </si>
-  <si>
-    <t>670928417-4</t>
-  </si>
-  <si>
-    <t>nam nulla integer pede justo lacinia eget tincidunt eget tempus vel pede morbi porttitor lorem id ligula</t>
-  </si>
-  <si>
-    <t>vestibulum ac est lacinia nisi venenatis tristique fusce congue diam id</t>
-  </si>
-  <si>
-    <t>dictumst etiam faucibus cursus urna ut tellus nulla ut erat id mauris vulputate elementum nullam varius nulla facilisi cras</t>
-  </si>
-  <si>
-    <t>12/28/2014</t>
   </si>
   <si>
     <t>In congue. Etiam justo. Etiam pretium iaculis justo.</t>
@@ -272,36 +152,126 @@
 Duis consequat dui nec nisi volutpat eleifend. Donec ut dolor. Morbi vel lectus in quam fringilla rhoncus.</t>
   </si>
   <si>
-    <t>330323769-7</t>
-  </si>
-  <si>
-    <t>mauris morbi non lectus aliquam sit amet diam in magna bibendum imperdiet nullam orci pede venenatis non sodales sed tincidunt</t>
-  </si>
-  <si>
-    <t>curae donec pharetra magna vestibulum aliquet ultrices erat tortor sollicitudin mi sit amet lobortis sapien sapien</t>
-  </si>
-  <si>
-    <t>sapien cursus vestibulum proin eu mi nulla ac enim in tempor turpis nec euismod scelerisque quam turpis adipiscing lorem</t>
-  </si>
-  <si>
-    <t>6/16/2014</t>
-  </si>
-  <si>
     <t>Suspendisse potenti. In eleifend quam a odio. In hac habitasse platea dictumst.</t>
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>eJx2T5970d</t>
+  </si>
+  <si>
+    <t>UnI30yCypM</t>
+  </si>
+  <si>
+    <t>UGuFgZz2nB</t>
+  </si>
+  <si>
+    <t>mAr8fxzX6q</t>
+  </si>
+  <si>
+    <t>C6Owxs8YoG</t>
+  </si>
+  <si>
+    <t>xp3sG3oZ3A</t>
+  </si>
+  <si>
+    <t>mPwwEjlCZz</t>
+  </si>
+  <si>
+    <t>y88nF1j3wX</t>
+  </si>
+  <si>
+    <t>kz3O3TjYoF</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>cDNA/mRNA</t>
+  </si>
+  <si>
+    <t>Whole blood</t>
+  </si>
+  <si>
+    <t>Serum</t>
+  </si>
+  <si>
+    <t>Cell lines</t>
+  </si>
+  <si>
+    <t>Urine</t>
+  </si>
+  <si>
+    <t>Faeces</t>
+  </si>
+  <si>
+    <t>liquid nitrogen freezer</t>
+  </si>
+  <si>
+    <t>sample box</t>
+  </si>
+  <si>
+    <t>vial box</t>
+  </si>
+  <si>
+    <t>blood box</t>
+  </si>
+  <si>
+    <t>breast tissue collection box</t>
+  </si>
+  <si>
+    <t>test tube</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>-18 °C to -35 °C</t>
+  </si>
+  <si>
+    <t>-60 °C to -85 °C</t>
+  </si>
+  <si>
+    <t>-60 °C to -85 °C</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>2 °C to 10°C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -324,14 +294,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -660,28 +640,28 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="101" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="346.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="99.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="346.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="99.875" bestFit="1" customWidth="1"/>
     <col min="18" max="22" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +683,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -749,7 +729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>65</v>
       </c>
@@ -760,19 +740,19 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="5">
+        <v>41734</v>
       </c>
       <c r="I2">
         <v>3563634990094343</v>
@@ -784,13 +764,13 @@
         <v>3563634990094343</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O2">
         <v>58</v>
@@ -799,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R2">
         <v>3563634990094343</v>
@@ -817,9 +797,9 @@
         <v>3563634990094343</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>80</v>
@@ -828,19 +808,19 @@
         <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="5">
+        <v>41905</v>
       </c>
       <c r="I3">
         <v>3544707904337273</v>
@@ -852,13 +832,13 @@
         <v>3544707904337273</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O3">
         <v>29</v>
@@ -867,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="Q3" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R3">
         <v>3544707904337273</v>
@@ -885,9 +865,9 @@
         <v>3544707904337273</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>44</v>
@@ -896,19 +876,19 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="5">
+        <v>40413</v>
       </c>
       <c r="I4">
         <v>3560783704165908</v>
@@ -920,13 +900,13 @@
         <v>3560783704165908</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O4">
         <v>6</v>
@@ -935,7 +915,7 @@
         <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R4">
         <v>3560783704165908</v>
@@ -953,9 +933,9 @@
         <v>3560783704165908</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>68</v>
@@ -966,17 +946,17 @@
       <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="5">
+        <v>41493</v>
       </c>
       <c r="I5">
         <v>3560432865281712</v>
@@ -988,13 +968,13 @@
         <v>3560432865281712</v>
       </c>
       <c r="L5" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O5">
         <v>78</v>
@@ -1003,7 +983,7 @@
         <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R5">
         <v>3560432865281712</v>
@@ -1021,7 +1001,7 @@
         <v>3560432865281712</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>97</v>
       </c>
@@ -1032,19 +1012,19 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H6" t="s">
-        <v>54</v>
+      <c r="F6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="5">
+        <v>38983</v>
       </c>
       <c r="I6">
         <v>6.7091304052969677E+18</v>
@@ -1056,13 +1036,13 @@
         <v>6.7091304052969677E+18</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O6">
         <v>84</v>
@@ -1071,7 +1051,7 @@
         <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R6">
         <v>6.7091304052969677E+18</v>
@@ -1089,9 +1069,9 @@
         <v>6.7091304052969677E+18</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>87</v>
@@ -1100,19 +1080,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>61</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="5">
+        <v>40444</v>
       </c>
       <c r="I7">
         <v>4.9118126066076662E+18</v>
@@ -1124,13 +1104,13 @@
         <v>4.9118126066076662E+18</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O7">
         <v>91</v>
@@ -1139,7 +1119,7 @@
         <v>38</v>
       </c>
       <c r="Q7" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R7">
         <v>4.9118126066076662E+18</v>
@@ -1157,7 +1137,7 @@
         <v>4.9118126066076662E+18</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>86</v>
       </c>
@@ -1168,19 +1148,19 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>68</v>
+      </c>
+      <c r="H8" s="5">
+        <v>42274</v>
       </c>
       <c r="I8">
         <v>5108756793765063</v>
@@ -1192,13 +1172,13 @@
         <v>5108756793765063</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="N8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O8">
         <v>36</v>
@@ -1207,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="Q8" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R8">
         <v>5108756793765063</v>
@@ -1225,7 +1205,7 @@
         <v>5108756793765063</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>44</v>
       </c>
@@ -1236,19 +1216,19 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" t="s">
-        <v>75</v>
+        <v>48</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="5">
+        <v>38147</v>
       </c>
       <c r="I9">
         <v>3578733792266993</v>
@@ -1260,13 +1240,13 @@
         <v>3578733792266993</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O9">
         <v>85</v>
@@ -1275,7 +1255,7 @@
         <v>43</v>
       </c>
       <c r="Q9" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R9">
         <v>3578733792266993</v>
@@ -1293,7 +1273,7 @@
         <v>3578733792266993</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>87</v>
       </c>
@@ -1304,19 +1284,19 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" t="s">
-        <v>83</v>
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="5">
+        <v>36781</v>
       </c>
       <c r="I10">
         <v>3584227658226946</v>
@@ -1328,13 +1308,13 @@
         <v>3584227658226946</v>
       </c>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="M10" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="N10" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O10">
         <v>73</v>
@@ -1343,7 +1323,7 @@
         <v>86</v>
       </c>
       <c r="Q10" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="R10">
         <v>3535602681713377</v>
@@ -1363,6 +1343,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
service.xml change for sample
</commit_message>
<xml_diff>
--- a/uploaded/MOCK_DATA_short.xlsx
+++ b/uploaded/MOCK_DATA_short.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15615" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="1" r:id="rId1"/>
+    <sheet name="sample" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
-  <si>
-    <t>sampleId</t>
-  </si>
-  <si>
-    <t>sampleCollectionDbId</t>
-  </si>
-  <si>
-    <t>biobankDbId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>hashedSampleId</t>
   </si>
@@ -54,9 +45,6 @@
     <t>anatomicalPartOntologyCode</t>
   </si>
   <si>
-    <t>anatomicalPartDescription</t>
-  </si>
-  <si>
     <t>anatomicalPartFreeText</t>
   </si>
   <si>
@@ -81,77 +69,30 @@
     <t>diseaseOntologyCode</t>
   </si>
   <si>
-    <t>diseaseDescription</t>
-  </si>
-  <si>
     <t>diseaseFreeText</t>
   </si>
   <si>
     <t>Aenean lectus. Pellentesque eget nunc. Donec quis orci eget orci vehicula condimentum.</t>
   </si>
   <si>
-    <t>Proin interdum mauris non ligula pellentesque ultrices. Phasellus id sapien in sapien iaculis congue. Vivamus metus arcu, adipiscing molestie, hendrerit at, vulputate vitae, nisl.</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>Quisque id justo sit amet sapien dignissim vestibulum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Nulla dapibus dolor vel est. Donec odio justo, sollicitudin ut, suscipit a, feugiat et, eros.
-Vestibulum ac est lacinia nisi venenatis tristique. Fusce congue, diam id ornare imperdiet, sapien urna pretium nisl, ut volutpat sapien arcu sed augue. Aliquam erat volutpat.
-In congue. Etiam justo. Etiam pretium iaculis justo.</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>Integer tincidunt ante vel ipsum. Praesent blandit lacinia erat. Vestibulum sed magna at nunc commodo placerat.
-Praesent blandit. Nam nulla. Integer pede justo, lacinia eget, tincidunt eget, tempus vel, pede.
-Morbi porttitor lorem id ligula. Suspendisse ornare consequat lectus. In est risus, auctor sed, tristique in, tempus sit amet, sem.</t>
-  </si>
-  <si>
-    <t>Nulla ut erat id mauris vulputate elementum. Nullam varius. Nulla facilisi.
-Cras non velit nec nisi vulputate nonummy. Maecenas tincidunt lacus at velit. Vivamus vel nulla eget eros elementum pellentesque.</t>
-  </si>
-  <si>
-    <t>Etiam vel augue. Vestibulum rutrum rutrum neque. Aenean auctor gravida sem.
-Praesent id massa id nisl venenatis lacinia. Aenean sit amet justo. Morbi ut odio.
-Cras mi pede, malesuada in, imperdiet et, commodo vulputate, justo. In blandit ultrices enim. Lorem ipsum dolor sit amet, consectetuer adipiscing elit.</t>
-  </si>
-  <si>
     <t>Curabitur in libero ut massa volutpat convallis. Morbi odio odio, elementum eu, interdum eu, tincidunt in, leo. Maecenas pulvinar lobortis est.</t>
   </si>
   <si>
     <t>Nullam porttitor lacus at turpis. Donec posuere metus vitae ipsum. Aliquam non mauris.</t>
   </si>
   <si>
-    <t>Maecenas tristique, est et tempus semper, est quam pharetra magna, ac consequat metus sapien ut nunc. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Mauris viverra diam vitae quam. Suspendisse potenti.
-Nullam porttitor lacus at turpis. Donec posuere metus vitae ipsum. Aliquam non mauris.</t>
-  </si>
-  <si>
-    <t>Praesent blandit. Nam nulla. Integer pede justo, lacinia eget, tincidunt eget, tempus vel, pede.
-Morbi porttitor lorem id ligula. Suspendisse ornare consequat lectus. In est risus, auctor sed, tristique in, tempus sit amet, sem.
-Fusce consequat. Nulla nisl. Nunc nisl.</t>
-  </si>
-  <si>
     <t>In quis justo. Maecenas rhoncus aliquam lacus. Morbi quis tortor id nulla ultrices aliquet.</t>
   </si>
   <si>
-    <t>In hac habitasse platea dictumst. Morbi vestibulum, velit id pretium iaculis, diam erat fermentum justo, nec condimentum neque sapien placerat ante. Nulla justo.</t>
-  </si>
-  <si>
     <t>In congue. Etiam justo. Etiam pretium iaculis justo.</t>
   </si>
   <si>
-    <t>In hac habitasse platea dictumst. Morbi vestibulum, velit id pretium iaculis, diam erat fermentum justo, nec condimentum neque sapien placerat ante. Nulla justo.
-Aliquam quis turpis eget elit sodales scelerisque. Mauris sit amet eros. Suspendisse accumsan tortor quis turpis.
-Sed ante. Vivamus tortor. Duis mattis egestas metus.</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Proin risus. Praesent lectus.
-Vestibulum quam sapien, varius ut, blandit non, interdum in, ante. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Duis faucibus accumsan odio. Curabitur convallis.
-Duis consequat dui nec nisi volutpat eleifend. Donec ut dolor. Morbi vel lectus in quam fringilla rhoncus.</t>
-  </si>
-  <si>
     <t>Suspendisse potenti. In eleifend quam a odio. In hac habitasse platea dictumst.</t>
   </si>
   <si>
@@ -240,16 +181,55 @@
   </si>
   <si>
     <t>2 °C to 10°C</t>
+  </si>
+  <si>
+    <t>Proin interdum mauris non ligula pellentesque ultrices.</t>
+  </si>
+  <si>
+    <t>Quisque id justo sit amet sapien dignissim vestibulum.</t>
+  </si>
+  <si>
+    <t>Nulla ut erat id mauris vulputate elementum. Nullam varius.</t>
+  </si>
+  <si>
+    <t>Integer tincidunt ante vel ipsum. Praesent blandit lacinia erat.</t>
+  </si>
+  <si>
+    <t>Praesent blandit. Nam nulla. Integer pede just.</t>
+  </si>
+  <si>
+    <t>In hac habitasse platea dictumst.</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit.</t>
+  </si>
+  <si>
+    <t>Etiam vel augue. Vestibulum rutrum rutrum neque.</t>
+  </si>
+  <si>
+    <t>Maecenas tristique, est et tempus semper, est quam pharetra magna, ac consequat metus sapien ut nun.</t>
+  </si>
+  <si>
+    <t>sampleCollectionId</t>
+  </si>
+  <si>
+    <t>biobankId</t>
+  </si>
+  <si>
+    <t>anatomicalPartOntologyDescription</t>
+  </si>
+  <si>
+    <t>diseaseOntologyDescription</t>
+  </si>
+  <si>
+    <t>sampleDbId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -273,6 +253,12 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,13 +280,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,94 +626,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="101" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="346.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="99.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="116.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -740,19 +735,19 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="5">
-        <v>41734</v>
+        <v>48</v>
+      </c>
+      <c r="H2" s="6">
+        <v>41161</v>
       </c>
       <c r="I2">
         <v>3563634990094343</v>
@@ -764,13 +759,13 @@
         <v>3563634990094343</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O2">
         <v>58</v>
@@ -779,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R2">
         <v>3563634990094343</v>
@@ -808,19 +803,19 @@
         <v>95</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="5">
-        <v>41905</v>
+        <v>49</v>
+      </c>
+      <c r="H3" s="6">
+        <v>41154</v>
       </c>
       <c r="I3">
         <v>3544707904337273</v>
@@ -832,13 +827,13 @@
         <v>3544707904337273</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O3">
         <v>29</v>
@@ -847,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="Q3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R3">
         <v>3544707904337273</v>
@@ -876,19 +871,19 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="5">
-        <v>40413</v>
+        <v>53</v>
+      </c>
+      <c r="H4" s="6">
+        <v>36527</v>
       </c>
       <c r="I4">
         <v>3560783704165908</v>
@@ -900,13 +895,13 @@
         <v>3560783704165908</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O4">
         <v>6</v>
@@ -915,7 +910,7 @@
         <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R4">
         <v>3560783704165908</v>
@@ -944,19 +939,19 @@
         <v>85</v>
       </c>
       <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="5">
-        <v>41493</v>
+        <v>53</v>
+      </c>
+      <c r="H5" s="6">
+        <v>39499</v>
       </c>
       <c r="I5">
         <v>3560432865281712</v>
@@ -968,13 +963,13 @@
         <v>3560432865281712</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O5">
         <v>78</v>
@@ -983,7 +978,7 @@
         <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R5">
         <v>3560432865281712</v>
@@ -1012,19 +1007,19 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="5">
-        <v>38983</v>
+        <v>50</v>
+      </c>
+      <c r="H6" s="6">
+        <v>39275</v>
       </c>
       <c r="I6">
         <v>6.7091304052969677E+18</v>
@@ -1036,13 +1031,13 @@
         <v>6.7091304052969677E+18</v>
       </c>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O6">
         <v>84</v>
@@ -1051,7 +1046,7 @@
         <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R6">
         <v>6.7091304052969677E+18</v>
@@ -1080,19 +1075,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="5">
-        <v>40444</v>
+        <v>51</v>
+      </c>
+      <c r="H7" s="6">
+        <v>39652</v>
       </c>
       <c r="I7">
         <v>4.9118126066076662E+18</v>
@@ -1104,13 +1099,13 @@
         <v>4.9118126066076662E+18</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="M7" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O7">
         <v>91</v>
@@ -1119,7 +1114,7 @@
         <v>38</v>
       </c>
       <c r="Q7" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R7">
         <v>4.9118126066076662E+18</v>
@@ -1148,19 +1143,19 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="5">
-        <v>42274</v>
+        <v>53</v>
+      </c>
+      <c r="H8" s="6">
+        <v>38333</v>
       </c>
       <c r="I8">
         <v>5108756793765063</v>
@@ -1172,13 +1167,13 @@
         <v>5108756793765063</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O8">
         <v>36</v>
@@ -1187,7 +1182,7 @@
         <v>3</v>
       </c>
       <c r="Q8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R8">
         <v>5108756793765063</v>
@@ -1216,19 +1211,19 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="5">
-        <v>38147</v>
+        <v>53</v>
+      </c>
+      <c r="H9" s="6">
+        <v>39805</v>
       </c>
       <c r="I9">
         <v>3578733792266993</v>
@@ -1240,13 +1235,13 @@
         <v>3578733792266993</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O9">
         <v>85</v>
@@ -1255,7 +1250,7 @@
         <v>43</v>
       </c>
       <c r="Q9" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R9">
         <v>3578733792266993</v>
@@ -1273,7 +1268,7 @@
         <v>3578733792266993</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>87</v>
       </c>
@@ -1284,19 +1279,19 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="5">
-        <v>36781</v>
+        <v>52</v>
+      </c>
+      <c r="H10" s="6">
+        <v>41161</v>
       </c>
       <c r="I10">
         <v>3584227658226946</v>
@@ -1308,13 +1303,13 @@
         <v>3584227658226946</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="M10" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O10">
         <v>73</v>
@@ -1323,7 +1318,7 @@
         <v>86</v>
       </c>
       <c r="Q10" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="R10">
         <v>3535602681713377</v>
@@ -1342,12 +1337,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="15" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sample upload possible with unordered column and gaps in excel template.
</commit_message>
<xml_diff>
--- a/uploaded/MOCK_DATA_short.xlsx
+++ b/uploaded/MOCK_DATA_short.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15615" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="525" windowWidth="25605" windowHeight="15555" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="2" r:id="rId1"/>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>